<commit_message>
adicionar columna en bases de datos
</commit_message>
<xml_diff>
--- a/002_sprints/004_sprint4/bosquejo_base_datos.xlsx
+++ b/002_sprints/004_sprint4/bosquejo_base_datos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="88">
   <si>
     <t xml:space="preserve">usuario</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">medico</t>
   </si>
   <si>
+    <t xml:space="preserve">Clave: 12345678</t>
+  </si>
+  <si>
     <t xml:space="preserve">id</t>
   </si>
   <si>
@@ -137,6 +140,12 @@
   </si>
   <si>
     <t xml:space="preserve">hora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disponible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">noDisponible</t>
   </si>
   <si>
     <t xml:space="preserve">citaMedica</t>
@@ -286,7 +295,7 @@
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="166" formatCode="hh:mm"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -307,11 +316,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -382,12 +386,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -399,19 +407,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -423,7 +423,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -506,11 +506,11 @@
   </sheetPr>
   <dimension ref="A2:X51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="17.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.98"/>
@@ -526,236 +526,244 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="H4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="3" t="n">
         <v>101534234</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="2" t="n">
+      <c r="F5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="3" t="n">
         <v>101434225</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="3" t="n">
+        <v>101434225</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="2" t="n">
-        <v>101434225</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="H6" s="3" t="n">
+        <v>1023434225</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="3" t="n">
+        <v>54683429</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="2" t="n">
-        <v>1023434225</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="2" t="n">
-        <v>54683429</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>11</v>
+      <c r="F7" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="H7" s="3" t="n">
         <v>123456789</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>17</v>
+      <c r="I7" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="3" t="n">
         <v>1023434225</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="C8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="3" t="n">
+        <v>102234234</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="2" t="n">
+      <c r="F9" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="3" t="n">
+        <v>123456789</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H13" s="3" t="n">
+        <v>101534234</v>
+      </c>
+      <c r="I13" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H14" s="3" t="n">
         <v>102234234</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="2" t="n">
-        <v>123456789</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H13" s="2" t="n">
-        <v>101534234</v>
-      </c>
-      <c r="I13" s="2" t="n">
+      <c r="I14" s="3" t="n">
+        <v>55</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H14" s="2" t="n">
-        <v>102234234</v>
-      </c>
-      <c r="I14" s="2" t="n">
-        <v>55</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>34</v>
+      <c r="M14" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="B18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="D18" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="E18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="2" t="n">
+      <c r="B19" s="3" t="n">
         <v>50</v>
       </c>
-      <c r="C19" s="2" t="n">
+      <c r="C19" s="3" t="n">
         <v>101434225</v>
       </c>
       <c r="D19" s="5" t="n">
@@ -764,13 +772,16 @@
       <c r="E19" s="6" t="n">
         <v>0.416666666666667</v>
       </c>
+      <c r="F19" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="2" t="n">
+      <c r="B20" s="3" t="n">
         <f aca="false">B19 +1</f>
         <v>51</v>
       </c>
-      <c r="C20" s="2" t="n">
+      <c r="C20" s="3" t="n">
         <v>101434225</v>
       </c>
       <c r="D20" s="5" t="n">
@@ -779,13 +790,17 @@
       <c r="E20" s="6" t="n">
         <v>0.4375</v>
       </c>
+      <c r="F20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="2" t="n">
+      <c r="B21" s="3" t="n">
         <f aca="false">B20 +1</f>
         <v>52</v>
       </c>
-      <c r="C21" s="2" t="n">
+      <c r="C21" s="3" t="n">
         <v>101434225</v>
       </c>
       <c r="D21" s="5" t="n">
@@ -794,13 +809,17 @@
       <c r="E21" s="6" t="n">
         <v>0.458333333333333</v>
       </c>
+      <c r="F21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H21" s="8"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="2" t="n">
+      <c r="B22" s="3" t="n">
         <f aca="false">B21 +1</f>
         <v>53</v>
       </c>
-      <c r="C22" s="2" t="n">
+      <c r="C22" s="3" t="n">
         <v>101434225</v>
       </c>
       <c r="D22" s="5" t="n">
@@ -809,13 +828,16 @@
       <c r="E22" s="6" t="n">
         <v>0.416666666666667</v>
       </c>
+      <c r="F22" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="2" t="n">
+      <c r="B23" s="3" t="n">
         <f aca="false">B22 +1</f>
         <v>54</v>
       </c>
-      <c r="C23" s="2" t="n">
+      <c r="C23" s="3" t="n">
         <v>101434225</v>
       </c>
       <c r="D23" s="5" t="n">
@@ -824,13 +846,16 @@
       <c r="E23" s="6" t="n">
         <v>0.4375</v>
       </c>
+      <c r="F23" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="2" t="n">
+      <c r="B24" s="3" t="n">
         <f aca="false">B23 +1</f>
         <v>55</v>
       </c>
-      <c r="C24" s="2" t="n">
+      <c r="C24" s="3" t="n">
         <v>101434225</v>
       </c>
       <c r="D24" s="5" t="n">
@@ -839,13 +864,16 @@
       <c r="E24" s="6" t="n">
         <v>0.458333333333333</v>
       </c>
+      <c r="F24" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="2" t="n">
+      <c r="B25" s="3" t="n">
         <f aca="false">B24 +1</f>
         <v>56</v>
       </c>
-      <c r="C25" s="2" t="n">
+      <c r="C25" s="3" t="n">
         <v>101434225</v>
       </c>
       <c r="D25" s="5" t="n">
@@ -854,13 +882,16 @@
       <c r="E25" s="6" t="n">
         <v>0.416666666666667</v>
       </c>
+      <c r="F25" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="2" t="n">
+      <c r="B26" s="3" t="n">
         <f aca="false">B25 +1</f>
         <v>57</v>
       </c>
-      <c r="C26" s="2" t="n">
+      <c r="C26" s="3" t="n">
         <v>101434225</v>
       </c>
       <c r="D26" s="5" t="n">
@@ -869,13 +900,16 @@
       <c r="E26" s="6" t="n">
         <v>0.4375</v>
       </c>
+      <c r="F26" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="2" t="n">
+      <c r="B27" s="3" t="n">
         <f aca="false">B26 +1</f>
         <v>58</v>
       </c>
-      <c r="C27" s="2" t="n">
+      <c r="C27" s="3" t="n">
         <v>101434225</v>
       </c>
       <c r="D27" s="5" t="n">
@@ -884,13 +918,16 @@
       <c r="E27" s="6" t="n">
         <v>0.458333333333333</v>
       </c>
+      <c r="F27" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="2" t="n">
+      <c r="B28" s="3" t="n">
         <f aca="false">B27 +1</f>
         <v>59</v>
       </c>
-      <c r="C28" s="2" t="n">
+      <c r="C28" s="3" t="n">
         <v>1023434225</v>
       </c>
       <c r="D28" s="5" t="n">
@@ -899,13 +936,16 @@
       <c r="E28" s="6" t="n">
         <v>0.416666666666667</v>
       </c>
+      <c r="F28" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="2" t="n">
+      <c r="B29" s="3" t="n">
         <f aca="false">B28 +1</f>
         <v>60</v>
       </c>
-      <c r="C29" s="2" t="n">
+      <c r="C29" s="3" t="n">
         <v>1023434225</v>
       </c>
       <c r="D29" s="5" t="n">
@@ -914,13 +954,16 @@
       <c r="E29" s="6" t="n">
         <v>0.4375</v>
       </c>
+      <c r="F29" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="2" t="n">
+      <c r="B30" s="3" t="n">
         <f aca="false">B29 +1</f>
         <v>61</v>
       </c>
-      <c r="C30" s="2" t="n">
+      <c r="C30" s="3" t="n">
         <v>1023434225</v>
       </c>
       <c r="D30" s="5" t="n">
@@ -929,13 +972,16 @@
       <c r="E30" s="6" t="n">
         <v>0.458333333333333</v>
       </c>
+      <c r="F30" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="2" t="n">
+      <c r="B31" s="3" t="n">
         <f aca="false">B30 +1</f>
         <v>62</v>
       </c>
-      <c r="C31" s="2" t="n">
+      <c r="C31" s="3" t="n">
         <v>1023434225</v>
       </c>
       <c r="D31" s="5" t="n">
@@ -944,13 +990,16 @@
       <c r="E31" s="6" t="n">
         <v>0.416666666666667</v>
       </c>
+      <c r="F31" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="2" t="n">
+      <c r="B32" s="3" t="n">
         <f aca="false">B31 +1</f>
         <v>63</v>
       </c>
-      <c r="C32" s="2" t="n">
+      <c r="C32" s="3" t="n">
         <v>1023434225</v>
       </c>
       <c r="D32" s="5" t="n">
@@ -959,13 +1008,16 @@
       <c r="E32" s="6" t="n">
         <v>0.4375</v>
       </c>
+      <c r="F32" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="2" t="n">
+      <c r="B33" s="3" t="n">
         <f aca="false">B32 +1</f>
         <v>64</v>
       </c>
-      <c r="C33" s="2" t="n">
+      <c r="C33" s="3" t="n">
         <v>1023434225</v>
       </c>
       <c r="D33" s="5" t="n">
@@ -974,13 +1026,16 @@
       <c r="E33" s="6" t="n">
         <v>0.458333333333333</v>
       </c>
+      <c r="F33" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="2" t="n">
+      <c r="B34" s="3" t="n">
         <f aca="false">B33 +1</f>
         <v>65</v>
       </c>
-      <c r="C34" s="2" t="n">
+      <c r="C34" s="3" t="n">
         <v>1023434225</v>
       </c>
       <c r="D34" s="5" t="n">
@@ -989,13 +1044,16 @@
       <c r="E34" s="6" t="n">
         <v>0.416666666666667</v>
       </c>
+      <c r="F34" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="2" t="n">
+      <c r="B35" s="3" t="n">
         <f aca="false">B34 +1</f>
         <v>66</v>
       </c>
-      <c r="C35" s="2" t="n">
+      <c r="C35" s="3" t="n">
         <v>1023434225</v>
       </c>
       <c r="D35" s="5" t="n">
@@ -1004,13 +1062,16 @@
       <c r="E35" s="6" t="n">
         <v>0.4375</v>
       </c>
+      <c r="F35" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="2" t="n">
+      <c r="B36" s="3" t="n">
         <f aca="false">B35 +1</f>
         <v>67</v>
       </c>
-      <c r="C36" s="2" t="n">
+      <c r="C36" s="3" t="n">
         <v>1023434225</v>
       </c>
       <c r="D36" s="5" t="n">
@@ -1019,320 +1080,323 @@
       <c r="E36" s="6" t="n">
         <v>0.458333333333333</v>
       </c>
+      <c r="F36" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
+      <c r="B41" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="2" t="n">
+      <c r="B42" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C42" s="2" t="n">
+      <c r="C42" s="3" t="n">
         <f aca="false">B25</f>
         <v>56</v>
       </c>
-      <c r="D42" s="2" t="n">
+      <c r="D42" s="3" t="n">
         <v>101534234</v>
       </c>
-      <c r="E42" s="2" t="n">
+      <c r="E42" s="3" t="n">
         <v>101434225</v>
       </c>
-      <c r="F42" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G42" s="2"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
+      <c r="F42" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G42" s="3"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="2" t="n">
+      <c r="B43" s="3" t="n">
         <f aca="false">B42 +1</f>
         <v>2</v>
       </c>
-      <c r="C43" s="2" t="n">
+      <c r="C43" s="3" t="n">
         <f aca="false">B33</f>
         <v>64</v>
       </c>
-      <c r="D43" s="2" t="n">
+      <c r="D43" s="3" t="n">
         <v>101534234</v>
       </c>
-      <c r="E43" s="2" t="n">
+      <c r="E43" s="3" t="n">
         <v>1023434225</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G43" s="2" t="n">
+      <c r="F43" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G43" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="2" t="n">
+      <c r="B44" s="3" t="n">
         <f aca="false">B43 +1</f>
         <v>3</v>
       </c>
-      <c r="C44" s="2" t="n">
+      <c r="C44" s="3" t="n">
         <f aca="false">B21</f>
         <v>52</v>
       </c>
-      <c r="D44" s="2" t="n">
+      <c r="D44" s="3" t="n">
         <v>101534234</v>
       </c>
-      <c r="E44" s="2" t="n">
+      <c r="E44" s="3" t="n">
         <v>101434225</v>
       </c>
-      <c r="F44" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G44" s="2"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="7"/>
+      <c r="F44" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G44" s="3"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="2" t="n">
+      <c r="B45" s="3" t="n">
         <f aca="false">B44 +1</f>
         <v>4</v>
       </c>
-      <c r="C45" s="2" t="n">
+      <c r="C45" s="3" t="n">
         <f aca="false">B32</f>
         <v>63</v>
       </c>
-      <c r="D45" s="2" t="n">
+      <c r="D45" s="3" t="n">
         <v>102234234</v>
       </c>
-      <c r="E45" s="2" t="n">
+      <c r="E45" s="3" t="n">
         <v>1023434225</v>
       </c>
-      <c r="F45" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G45" s="2" t="n">
+      <c r="F45" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G45" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="H45" s="7"/>
-      <c r="I45" s="7"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="7"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="9"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K49" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L49" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M49" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N49" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O49" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="P49" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q49" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="R49" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="S49" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="T49" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="U49" s="9"/>
+      <c r="V49" s="9"/>
+      <c r="W49" s="9"/>
+      <c r="X49" s="9"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="C50" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="K49" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="L49" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="M49" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="N49" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="O49" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="P49" s="2" t="s">
+      <c r="D50" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="Q49" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="R49" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="S49" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="T49" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="U49" s="7"/>
-      <c r="V49" s="7"/>
-      <c r="W49" s="7"/>
-      <c r="X49" s="7"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="B50" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="C50" s="2" t="n">
+      <c r="J50" s="3" t="n">
+        <v>168</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="L50" s="3" t="n">
+        <v>35.5</v>
+      </c>
+      <c r="M50" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="N50" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="O50" s="3"/>
+      <c r="P50" s="3"/>
+      <c r="Q50" s="3"/>
+      <c r="R50" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="S50" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="T50" s="3"/>
+      <c r="U50" s="9"/>
+      <c r="V50" s="9"/>
+      <c r="W50" s="9"/>
+      <c r="X50" s="9"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" s="3" t="n">
+        <v>101</v>
+      </c>
+      <c r="C51" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I51" s="3" t="n">
+        <v>70</v>
+      </c>
+      <c r="J51" s="3" t="n">
+        <v>178</v>
+      </c>
+      <c r="K51" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="L51" s="3" t="n">
+        <v>37</v>
+      </c>
+      <c r="M51" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="N51" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2" t="n">
-        <v>60</v>
-      </c>
-      <c r="J50" s="2" t="n">
-        <v>168</v>
-      </c>
-      <c r="K50" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="L50" s="2" t="n">
-        <v>35.5</v>
-      </c>
-      <c r="M50" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="N50" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="O50" s="2"/>
-      <c r="P50" s="2"/>
-      <c r="Q50" s="2"/>
-      <c r="R50" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="S50" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="T50" s="2"/>
-      <c r="U50" s="7"/>
-      <c r="V50" s="7"/>
-      <c r="W50" s="7"/>
-      <c r="X50" s="7"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="B51" s="2" t="n">
-        <v>101</v>
-      </c>
-      <c r="C51" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I51" s="2" t="n">
-        <v>70</v>
-      </c>
-      <c r="J51" s="2" t="n">
-        <v>178</v>
-      </c>
-      <c r="K51" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="L51" s="2" t="n">
-        <v>37</v>
-      </c>
-      <c r="M51" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="N51" s="2" t="n">
+      <c r="O51" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="O51" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="P51" s="2" t="n">
+      <c r="P51" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="Q51" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="R51" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="S51" s="2"/>
-      <c r="T51" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="U51" s="7"/>
-      <c r="V51" s="7"/>
-      <c r="W51" s="7"/>
-      <c r="X51" s="7"/>
+      <c r="Q51" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="R51" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="S51" s="3"/>
+      <c r="T51" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U51" s="9"/>
+      <c r="V51" s="9"/>
+      <c r="W51" s="9"/>
+      <c r="X51" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>